<commit_message>
Added manual point selection
</commit_message>
<xml_diff>
--- a/BlueDrop_Calibration_Factors.xlsx
+++ b/BlueDrop_Calibration_Factors.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Geotech_Research\Field_Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Geotech_Research\Field_Analysis\BlueDrop_Analysis_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1076D3A-2F17-4D5D-939E-C5D53EC491CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F8A13D-E858-43BA-9A23-7381236B6F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ED08122E-F907-40EC-B515-5B3584CD96BD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="4" activeTab="4" xr2:uid="{ED08122E-F907-40EC-B515-5B3584CD96BD}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="4" r:id="rId1"/>
     <sheet name="bluedrop_1" sheetId="1" r:id="rId2"/>
     <sheet name="bluedrop_2" sheetId="2" r:id="rId3"/>
     <sheet name="bluedrop_3" sheetId="3" r:id="rId4"/>
+    <sheet name="bluedrop_9" sheetId="5" r:id="rId5"/>
+    <sheet name="copy" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="19">
   <si>
     <t>pore_pressure</t>
   </si>
@@ -103,12 +105,18 @@
   <si>
     <t>Sensor</t>
   </si>
+  <si>
+    <t>October_2023_offset</t>
+  </si>
+  <si>
+    <t>October_2023_scale</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -134,6 +142,27 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -152,10 +181,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -166,9 +196,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{2B3DE36A-4749-4829-AE03-A61F42EA842D}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -502,7 +537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EAFC28-FDDC-4734-9491-B8FE19884229}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -779,7 +814,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -891,4 +926,358 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2806BE-D5DA-4A6A-A258-3571B4D66185}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.69921875" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="5">
+        <v>-17196.900000000001</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1626262.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5">
+        <v>27399.599999999999</v>
+      </c>
+      <c r="C3" s="5">
+        <v>159870.39999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5">
+        <v>-246643.4</v>
+      </c>
+      <c r="C4" s="5">
+        <v>63690.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>16353.5</v>
+      </c>
+      <c r="C5" s="5">
+        <v>27604.799999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5">
+        <v>-8819.9</v>
+      </c>
+      <c r="C6" s="5">
+        <v>13630.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5">
+        <v>-16510</v>
+      </c>
+      <c r="C7" s="5">
+        <v>65260.800000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5">
+        <v>71742.600000000006</v>
+      </c>
+      <c r="C8" s="5">
+        <v>65778.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="5">
+        <v>17912.7</v>
+      </c>
+      <c r="C9" s="5">
+        <v>20278.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D17" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3ACE2B0-30A1-4BB2-93F0-875CB7C585E7}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.69921875" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="5">
+        <v>17196.900000000001</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1626262.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5">
+        <v>-27399.599999999999</v>
+      </c>
+      <c r="C3" s="5">
+        <v>159870.39999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5">
+        <v>246643.4</v>
+      </c>
+      <c r="C4" s="5">
+        <v>63690.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>-16353.5</v>
+      </c>
+      <c r="C5" s="5">
+        <v>27604.799999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5">
+        <v>8819.9</v>
+      </c>
+      <c r="C6" s="5">
+        <v>13630.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5">
+        <v>16510</v>
+      </c>
+      <c r="C7" s="5">
+        <v>65260.800000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5">
+        <v>-71742.600000000006</v>
+      </c>
+      <c r="C8" s="5">
+        <v>65778.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="5">
+        <v>-17912.7</v>
+      </c>
+      <c r="C9" s="5">
+        <v>20278.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <f>B2*-1</f>
+        <v>-17196.900000000001</v>
+      </c>
+      <c r="C12">
+        <f>C2*-1</f>
+        <v>-1626262.4</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <f t="shared" ref="B13:C19" si="0">B3*-1</f>
+        <v>27399.599999999999</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>-159870.39999999999</v>
+      </c>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>-246643.4</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>-63690.9</v>
+      </c>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>16353.5</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>-27604.799999999999</v>
+      </c>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>-8819.9</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>-13630.9</v>
+      </c>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>-16510</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>-65260.800000000003</v>
+      </c>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>71742.600000000006</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>-65778.7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>17912.7</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>-20278.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added bearing capacity calculation functions
</commit_message>
<xml_diff>
--- a/BlueDrop_Calibration_Factors.xlsx
+++ b/BlueDrop_Calibration_Factors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Geotech_Research\Field_Analysis\BlueDrop_Analysis_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F8A13D-E858-43BA-9A23-7381236B6F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C25091-E3EC-4063-91B9-93AB7C530B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="4" activeTab="4" xr2:uid="{ED08122E-F907-40EC-B515-5B3584CD96BD}"/>
+    <workbookView xWindow="-29640" yWindow="1605" windowWidth="17280" windowHeight="8970" xr2:uid="{ED08122E-F907-40EC-B515-5B3584CD96BD}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="bluedrop_2" sheetId="2" r:id="rId3"/>
     <sheet name="bluedrop_3" sheetId="3" r:id="rId4"/>
     <sheet name="bluedrop_9" sheetId="5" r:id="rId5"/>
-    <sheet name="copy" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
   <si>
     <t>pore_pressure</t>
   </si>
@@ -537,7 +536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EAFC28-FDDC-4734-9491-B8FE19884229}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -932,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2806BE-D5DA-4A6A-A258-3571B4D66185}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1069,215 +1068,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3ACE2B0-30A1-4BB2-93F0-875CB7C585E7}">
-  <dimension ref="A1:D19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:C19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.69921875" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="5">
-        <v>17196.900000000001</v>
-      </c>
-      <c r="C2" s="5">
-        <v>1626262.4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="5">
-        <v>-27399.599999999999</v>
-      </c>
-      <c r="C3" s="5">
-        <v>159870.39999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="5">
-        <v>246643.4</v>
-      </c>
-      <c r="C4" s="5">
-        <v>63690.9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5">
-        <v>-16353.5</v>
-      </c>
-      <c r="C5" s="5">
-        <v>27604.799999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="5">
-        <v>8819.9</v>
-      </c>
-      <c r="C6" s="5">
-        <v>13630.9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="5">
-        <v>16510</v>
-      </c>
-      <c r="C7" s="5">
-        <v>65260.800000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="5">
-        <v>-71742.600000000006</v>
-      </c>
-      <c r="C8" s="5">
-        <v>65778.7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="5">
-        <v>-17912.7</v>
-      </c>
-      <c r="C9" s="5">
-        <v>20278.7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B12">
-        <f>B2*-1</f>
-        <v>-17196.900000000001</v>
-      </c>
-      <c r="C12">
-        <f>C2*-1</f>
-        <v>-1626262.4</v>
-      </c>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B13">
-        <f t="shared" ref="B13:C19" si="0">B3*-1</f>
-        <v>27399.599999999999</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>-159870.39999999999</v>
-      </c>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>-246643.4</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>-63690.9</v>
-      </c>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>16353.5</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>-27604.799999999999</v>
-      </c>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>-8819.9</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>-13630.9</v>
-      </c>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>-16510</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
-        <v>-65260.800000000003</v>
-      </c>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>71742.600000000006</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="0"/>
-        <v>-65778.7</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>17912.7</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="0"/>
-        <v>-20278.7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>